<commit_message>
Updated dataloader to use IMF Data API
</commit_message>
<xml_diff>
--- a/weo_data_oct_2020.xlsx
+++ b/weo_data_oct_2020.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{53D6EBF1-F5F8-4CF8-9A04-64BEBE77E543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_data_oct_2020" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1136,11 +1136,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -8557,6 +8557,66 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AppVersion xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Invited_Teachers xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <FolderType xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Teachers xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Student_Groups xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Math_Settings xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <NotebookType xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Students xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <TeamsChannelId xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Invited_Students xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Owner xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Is_Collaboration_Space_Locked xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Templates xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <LMS_Mappings xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <CultureName xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+    <Distribution_Groups xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B6A43E5FE8F8B14A8BFE7C9ECF27E972" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1dfeb30582f02e12450726f3eaaeec07">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="15000dae-19c9-4482-aa88-2603c3e78971" xmlns:ns4="237e942f-dbc2-4015-82fa-37b450855f40" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7ef073190e711ba201c2a457c021e99" ns3:_="" ns4:_="">
     <xsd:import namespace="15000dae-19c9-4482-aa88-2603c3e78971"/>
@@ -8967,67 +9027,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1582DDBD-EF92-4380-B071-90CF9989CB8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="237e942f-dbc2-4015-82fa-37b450855f40"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="15000dae-19c9-4482-aa88-2603c3e78971"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AppVersion xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Invited_Teachers xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <FolderType xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Teachers xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Student_Groups xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Math_Settings xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <NotebookType xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Students xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <TeamsChannelId xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Invited_Students xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Owner xmlns="15000dae-19c9-4482-aa88-2603c3e78971">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Is_Collaboration_Space_Locked xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Templates xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <LMS_Mappings xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <CultureName xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-    <Distribution_Groups xmlns="15000dae-19c9-4482-aa88-2603c3e78971" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DCAED15-CCB6-4BF7-A9E6-24E9A59E6CFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF138F84-8D74-432B-9859-F76F79EBD319}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9044,29 +9069,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DCAED15-CCB6-4BF7-A9E6-24E9A59E6CFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1582DDBD-EF92-4380-B071-90CF9989CB8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="237e942f-dbc2-4015-82fa-37b450855f40"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="15000dae-19c9-4482-aa88-2603c3e78971"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>